<commit_message>
created a few extra excel tables to compare the results of different experiments
</commit_message>
<xml_diff>
--- a/Evaluation/gyroscope_vs_accelerometer.xlsx
+++ b/Evaluation/gyroscope_vs_accelerometer.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\redma\Documents\GitHub\ExerciseClassification\Evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Github\ExerciseClassification\Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265F91B4-6AD3-457A-A74F-1208C2112D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AF0D6E-A7D6-4CC3-8CD7-B88CD8DB092A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2970" yWindow="1875" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Mean Accuracy</t>
   </si>
@@ -85,13 +86,22 @@
   </si>
   <si>
     <t>Weighted</t>
+  </si>
+  <si>
+    <t>Accel and Gyro</t>
+  </si>
+  <si>
+    <t>Gyro</t>
+  </si>
+  <si>
+    <t>Accel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,8 +124,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.6"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color rgb="FFFF0000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +157,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -156,12 +194,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,22 +507,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -529,7 +592,7 @@
         <v>0.985164835164835</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -564,7 +627,7 @@
         <v>0.97087912087911998</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -599,7 +662,7 @@
         <v>0.99285714285714199</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -634,7 +697,7 @@
         <v>0.85277777777777697</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -669,7 +732,7 @@
         <v>0.84722222222222199</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -704,7 +767,7 @@
         <v>0.94166666666666599</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -739,7 +802,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -774,7 +837,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -807,6 +870,179 @@
       </c>
       <c r="K10" s="3">
         <v>0.938888888888888</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26DE2E46-6FBB-476F-A619-75D1BC428275}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.177777778</v>
+      </c>
+      <c r="C2" s="11">
+        <v>0.23611111100000001</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.19166666700000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.93333333299999999</v>
+      </c>
+      <c r="C3" s="12">
+        <v>0.95277777799999996</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0.97777777799999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.436111111</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0.47222222200000002</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.43333333299999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.96666666700000003</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.96944444399999996</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.97777777799999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0.82777777799999996</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.74444444399999998</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.85833333300000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12">
+        <v>0.66666666699999999</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.63333333300000005</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.70555555599999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12">
+        <v>0.66111111099999997</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.60833333300000003</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.76111111099999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.76111111099999995</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0.78333333299999997</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.82222222199999995</v>
+      </c>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12">
+        <v>0.98888888900000005</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.98333333300000003</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.99166666699999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13">
+        <v>0.85277777777777697</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.84722222222222199</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.94166666666666599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>